<commit_message>
Menambahkan fitur import data siswa dari file Excel.
</commit_message>
<xml_diff>
--- a/public/docs/FormatDataSiswa.xlsx
+++ b/public/docs/FormatDataSiswa.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>id_siswa</t>
   </si>
@@ -82,12 +82,90 @@
   </si>
   <si>
     <t>telp_wali</t>
+  </si>
+  <si>
+    <t>Arvindha Pramudya</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>Islam</t>
+  </si>
+  <si>
+    <t>Jl.Taman Bekasi Asri No.35</t>
+  </si>
+  <si>
+    <t>Iswidiyanto</t>
+  </si>
+  <si>
+    <t>Hernawati</t>
+  </si>
+  <si>
+    <t>Carissa Astrid Alissya</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Ciamis</t>
+  </si>
+  <si>
+    <t>Jl.Pariwisata 2 No.12A</t>
+  </si>
+  <si>
+    <t>Asep Adang Rustiawan</t>
+  </si>
+  <si>
+    <t>Elis Faridah</t>
+  </si>
+  <si>
+    <t>Fabian Noval Putra</t>
+  </si>
+  <si>
+    <t>Bekasi</t>
+  </si>
+  <si>
+    <t>Jl.Borobudur Blok 6 No.11</t>
+  </si>
+  <si>
+    <t>Tony Hamidi</t>
+  </si>
+  <si>
+    <t>Sri Mulyati</t>
+  </si>
+  <si>
+    <t>518131351</t>
+  </si>
+  <si>
+    <t>248218413</t>
+  </si>
+  <si>
+    <t>518131350</t>
+  </si>
+  <si>
+    <t>PNS</t>
+  </si>
+  <si>
+    <t>SAD</t>
+  </si>
+  <si>
+    <t>SDF</t>
+  </si>
+  <si>
+    <t>dsafs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -583,9 +661,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -941,31 +1020,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1"/>
@@ -1037,6 +1116,135 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2">
+        <v>6153135813</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="2">
+        <v>38341</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q2">
+        <v>12345678912</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3">
+        <v>3581381463</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2204</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3">
+        <v>12345678912</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>3513814381</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="2">
+        <v>38032</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q4">
+        <v>12345678912</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Memperbarui format impor data siswa.
</commit_message>
<xml_diff>
--- a/public/docs/FormatDataSiswa.xlsx
+++ b/public/docs/FormatDataSiswa.xlsx
@@ -18,6 +18,364 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Adnan Zaki</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adnan Zaki:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Hanya diisi angka
+- Wajib diisi
+- Harus unik</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adnan Zaki:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Hanya diisi angka
+- Wajib diisi
+- Harus unik</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adnan Zaki:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Wajib diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adnan Zaki:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Wajib diisi
+- Hanya diisi "L" atau "P"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adnan Zaki:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Wajib diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adnan Zaki:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Wajib diisi
+- Format harus YYYY-MM-DD
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adnan Zaki:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Wajib diisi
+- Hanya boleh diisi Islam, Katholik, Kristen Protestan, Hindu, Buddha</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adnan Zaki:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Wajib diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adnan Zaki:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Wajib diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adnan Zaki:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Wajib diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adnan Zaki:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Wajib diisi
+- Hanya boleh diisi PNS, Karyawan Swasta, Wiraswasta, Buruh, Tidak Bekerja, Lain-lain</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adnan Zaki:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Wajib diisi
+- Hanya boleh diisi PNS, Karyawan Swasta, Wiraswasta, Buruh, Ibu Rumah Tangga, Lain-lain</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adnan Zaki:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Wajib diisi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adnan Zaki:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+- Wajib diisi
+- Hanya boleh diisi angka
+- Minimal 11 karakter, maksimal 15 karakter</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
@@ -166,7 +524,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,6 +676,19 @@
       <family val="2"/>
       <charset val="1"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1019,11 +1390,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,5 +1620,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>